<commit_message>
Graphs Apriori_ correction on a title
</commit_message>
<xml_diff>
--- a/Reports/Apriori.xlsx
+++ b/Reports/Apriori.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ALESSANDRA\poli\5° ANNO\MINING PATTERNS IN DATA\ProjectsOfMiningPatternsInData\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A46657-9A0E-4A74-A8A4-C9F9A66BE4CB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97E93A4-3ADD-4121-A4F0-435061EAF8E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4860" xr2:uid="{93FA775B-083D-41A1-978D-664E19CBC73C}"/>
   </bookViews>
@@ -114,12 +114,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1149,7 +1149,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1162,14 +1162,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT"/>
+              <a:rPr lang="it-IT" u="sng"/>
               <a:t>Apriori performances</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="it-IT" baseline="0"/>
+              <a:rPr lang="it-IT" u="sng" baseline="0"/>
               <a:t> - MEMORY</a:t>
             </a:r>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="it-IT" u="sng"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1177,8 +1177,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.55938192383883178"/>
-          <c:y val="2.5225225225225224E-2"/>
+          <c:x val="0.24808009209285778"/>
+          <c:y val="1.4414414414414415E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1194,7 +1194,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3700,7 +3700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFCE8AF4-53E6-4F57-8D73-F5D41590ACF4}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
@@ -3721,41 +3721,41 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1" t="s">
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3823,7 +3823,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>0.95</v>
       </c>
       <c r="B4">
@@ -3888,7 +3888,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>0.89999999999999902</v>
       </c>
       <c r="B5">
@@ -3953,7 +3953,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>0.84999999999999898</v>
       </c>
       <c r="B6">
@@ -4018,7 +4018,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>0.79999999999999905</v>
       </c>
       <c r="B7">
@@ -4083,7 +4083,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>0.749999999999999</v>
       </c>
       <c r="B8">
@@ -4139,7 +4139,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>0.7</v>
       </c>
       <c r="B9">
@@ -4186,7 +4186,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>0.64999999999999902</v>
       </c>
       <c r="B10">
@@ -4233,7 +4233,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>0.59999999999999898</v>
       </c>
       <c r="B11">
@@ -4280,7 +4280,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>0.54999999999999905</v>
       </c>
       <c r="B12">
@@ -4327,7 +4327,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>0.499999999999999</v>
       </c>
       <c r="B13">
@@ -4374,7 +4374,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>0.44999999999999901</v>
       </c>
       <c r="B14">
@@ -4421,7 +4421,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>0.39999999999999902</v>
       </c>
       <c r="B15">
@@ -4617,135 +4617,135 @@
       </c>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H25" s="3"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>0.75</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <v>129</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="1">
         <v>20717000</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="1">
         <v>0.75</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="1">
         <v>1047</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="1">
         <v>15252440</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="1">
         <v>0.75</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="1">
         <v>628</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="1">
         <v>10131936</v>
       </c>
     </row>
     <row r="32" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>0.7</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>113</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="1">
         <v>2333384</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
         <v>0.7</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
         <v>1068</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="1">
         <v>23587624</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="1">
         <v>0.7</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="1">
         <v>600</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="1">
         <v>52455888</v>
       </c>
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>0.35</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>602</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="1">
         <v>36092080</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="1">
         <v>0.4</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="1">
         <v>1225</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="1">
         <v>9955936</v>
       </c>
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>0.3</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <v>957</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="1">
         <v>30078640</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="1">
         <v>0.35</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1">
         <v>535</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="1">
         <v>19135392</v>
       </c>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>0.25</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="1">
         <v>2158</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="1">
         <v>83981144</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="1">
         <v>0.3</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="1">
         <v>584</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L35" s="1">
         <v>9173712</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>